<commit_message>
added data for indicators
</commit_message>
<xml_diff>
--- a/deaths.xlsx
+++ b/deaths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Downloads/covid19-vuln/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Documents/covid19-vuln/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D89B8E-80E9-F941-BC06-C5B96706E557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7D7D9B-CA30-5B45-AAD2-4692D508F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3880" yWindow="460" windowWidth="24920" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="20">
   <si>
     <t>region</t>
   </si>
@@ -34,57 +34,6 @@
     <t>Arecibo</t>
   </si>
   <si>
-    <t>20 to 24</t>
-  </si>
-  <si>
-    <t>25 to 29</t>
-  </si>
-  <si>
-    <t>30 to 34</t>
-  </si>
-  <si>
-    <t>35 to 39</t>
-  </si>
-  <si>
-    <t>40 to 44</t>
-  </si>
-  <si>
-    <t>45 to 49</t>
-  </si>
-  <si>
-    <t>50 to 54</t>
-  </si>
-  <si>
-    <t>55 to 59</t>
-  </si>
-  <si>
-    <t>60 to 64</t>
-  </si>
-  <si>
-    <t>65 to 69</t>
-  </si>
-  <si>
-    <t>70 to 74</t>
-  </si>
-  <si>
-    <t>75 to 79</t>
-  </si>
-  <si>
-    <t>80 to 84</t>
-  </si>
-  <si>
-    <t>85 to 89</t>
-  </si>
-  <si>
-    <t>90 to 94</t>
-  </si>
-  <si>
-    <t>95 to 99</t>
-  </si>
-  <si>
-    <t>100 to 104</t>
-  </si>
-  <si>
     <t>Bayamon</t>
   </si>
   <si>
@@ -92,12 +41,6 @@
   </si>
   <si>
     <t>Fajardo</t>
-  </si>
-  <si>
-    <t>5 to 9</t>
-  </si>
-  <si>
-    <t>15 to 19</t>
   </si>
   <si>
     <t>Mayaguez</t>
@@ -470,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -494,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -505,7 +448,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -516,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -527,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -538,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>23</v>
@@ -549,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>51</v>
@@ -560,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>104</v>
@@ -571,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>139</v>
@@ -582,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>155</v>
@@ -590,21 +533,21 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -612,565 +555,670 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C16">
-        <v>117</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>162</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C18">
-        <v>220</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>295</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C23">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>81</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>97</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>155</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>212</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C33">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C34">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C35">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C36">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C37">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C42">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46">
         <v>26</v>
-      </c>
-      <c r="B46" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>18</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55">
         <v>27</v>
       </c>
-      <c r="B55" t="s">
-        <v>36</v>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C62">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C63">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C64">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C65">
-        <v>48</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66">
         <v>14</v>
-      </c>
-      <c r="C66">
-        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C67">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C68">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C69">
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70">
-        <v>30</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -1178,519 +1226,90 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C76">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C77">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C78">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C79">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C80">
-        <v>73</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C81">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>27</v>
-      </c>
-      <c r="B82" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B83" t="s">
-        <v>13</v>
-      </c>
-      <c r="C83">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>27</v>
-      </c>
-      <c r="B84" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>27</v>
-      </c>
-      <c r="B85" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>27</v>
-      </c>
-      <c r="B86" t="s">
-        <v>16</v>
-      </c>
-      <c r="C86">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>27</v>
-      </c>
-      <c r="B87" t="s">
-        <v>17</v>
-      </c>
-      <c r="C87">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>27</v>
-      </c>
-      <c r="B88" t="s">
-        <v>18</v>
-      </c>
-      <c r="C88">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>27</v>
-      </c>
-      <c r="B89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>27</v>
-      </c>
-      <c r="B90" t="s">
-        <v>20</v>
-      </c>
-      <c r="C90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>28</v>
-      </c>
-      <c r="B91" t="s">
-        <v>25</v>
-      </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>28</v>
-      </c>
-      <c r="B92" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>28</v>
-      </c>
-      <c r="B93" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>28</v>
-      </c>
-      <c r="B94" t="s">
-        <v>9</v>
-      </c>
-      <c r="C94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>28</v>
-      </c>
-      <c r="B95" t="s">
-        <v>10</v>
-      </c>
-      <c r="C95">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>28</v>
-      </c>
-      <c r="B96" t="s">
-        <v>11</v>
-      </c>
-      <c r="C96">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>28</v>
-      </c>
-      <c r="B97" t="s">
-        <v>12</v>
-      </c>
-      <c r="C97">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>28</v>
-      </c>
-      <c r="B98" t="s">
-        <v>13</v>
-      </c>
-      <c r="C98">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>28</v>
-      </c>
-      <c r="B99" t="s">
-        <v>14</v>
-      </c>
-      <c r="C99">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>28</v>
-      </c>
-      <c r="B100" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>28</v>
-      </c>
-      <c r="B101" t="s">
-        <v>16</v>
-      </c>
-      <c r="C101">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>28</v>
-      </c>
-      <c r="B102" t="s">
-        <v>18</v>
-      </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>29</v>
-      </c>
-      <c r="B103" t="s">
-        <v>24</v>
-      </c>
-      <c r="C103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>29</v>
-      </c>
-      <c r="B104" t="s">
-        <v>25</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>29</v>
-      </c>
-      <c r="B105" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>29</v>
-      </c>
-      <c r="B106" t="s">
-        <v>6</v>
-      </c>
-      <c r="C106">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>29</v>
-      </c>
-      <c r="B107" t="s">
-        <v>7</v>
-      </c>
-      <c r="C107">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>29</v>
-      </c>
-      <c r="B108" t="s">
-        <v>8</v>
-      </c>
-      <c r="C108">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>29</v>
-      </c>
-      <c r="B109" t="s">
-        <v>9</v>
-      </c>
-      <c r="C109">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>29</v>
-      </c>
-      <c r="B110" t="s">
-        <v>10</v>
-      </c>
-      <c r="C110">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>29</v>
-      </c>
-      <c r="B111" t="s">
-        <v>11</v>
-      </c>
-      <c r="C111">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>29</v>
-      </c>
-      <c r="B112" t="s">
-        <v>12</v>
-      </c>
-      <c r="C112">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>29</v>
-      </c>
-      <c r="B113" t="s">
-        <v>13</v>
-      </c>
-      <c r="C113">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>29</v>
-      </c>
-      <c r="B114" t="s">
-        <v>14</v>
-      </c>
-      <c r="C114">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>29</v>
-      </c>
-      <c r="B115" t="s">
-        <v>15</v>
-      </c>
-      <c r="C115">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>29</v>
-      </c>
-      <c r="B116" t="s">
-        <v>16</v>
-      </c>
-      <c r="C116">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>29</v>
-      </c>
-      <c r="B117" t="s">
-        <v>17</v>
-      </c>
-      <c r="C117">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>29</v>
-      </c>
-      <c r="B118" t="s">
-        <v>18</v>
-      </c>
-      <c r="C118">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>29</v>
-      </c>
-      <c r="B119" t="s">
-        <v>19</v>
-      </c>
-      <c r="C119">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>29</v>
-      </c>
-      <c r="B120" t="s">
-        <v>20</v>
-      </c>
-      <c r="C120">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing problem with special characters in municipality names
</commit_message>
<xml_diff>
--- a/deaths.xlsx
+++ b/deaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Documents/covid19-vuln/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7D7D9B-CA30-5B45-AAD2-4692D508F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C407B265-4DDE-0849-BC56-F0C75E1A0285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="460" windowWidth="24920" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11240" yWindow="460" windowWidth="17560" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="18">
   <si>
     <t>region</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Ponce</t>
   </si>
   <si>
-    <t>20 to 29</t>
-  </si>
-  <si>
     <t>30 to 39</t>
   </si>
   <si>
@@ -76,10 +73,7 @@
     <t>80+</t>
   </si>
   <si>
-    <t>0 to 9</t>
-  </si>
-  <si>
-    <t>10 to 19</t>
+    <t>0 to 29</t>
   </si>
 </sst>
 </file>
@@ -413,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="161" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -437,10 +431,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -448,10 +442,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -459,10 +453,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -470,10 +464,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -481,10 +475,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>23</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -492,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>51</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -503,10 +497,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>104</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -514,32 +508,32 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>139</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10">
-        <v>155</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,10 +541,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -558,10 +552,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -569,10 +563,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,10 +574,10 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>18</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,10 +585,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>39</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -602,54 +596,54 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18">
-        <v>162</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>220</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C20">
-        <v>295</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -657,10 +651,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -668,10 +662,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,10 +673,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -690,76 +684,76 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
         <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26">
-        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>81</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>97</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>155</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>212</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -767,10 +761,10 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,18 +772,18 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -797,73 +791,73 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C36">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38">
-        <v>33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39">
-        <v>40</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40">
-        <v>52</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
@@ -874,442 +868,255 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46">
-        <v>26</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C47">
-        <v>51</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <v>88</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
       </c>
       <c r="C50">
-        <v>187</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>12</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>27</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>79</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C57">
-        <v>143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C58">
-        <v>203</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C59">
-        <v>282</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C60">
-        <v>388</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65">
         <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" t="s">
-        <v>14</v>
-      </c>
-      <c r="C67">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" t="s">
-        <v>15</v>
-      </c>
-      <c r="C68">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" t="s">
-        <v>18</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" t="s">
-        <v>19</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>9</v>
-      </c>
-      <c r="B75" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>9</v>
-      </c>
-      <c r="B76" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" t="s">
-        <v>14</v>
-      </c>
-      <c r="C77">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>9</v>
-      </c>
-      <c r="B78" t="s">
-        <v>15</v>
-      </c>
-      <c r="C78">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" t="s">
-        <v>16</v>
-      </c>
-      <c r="C79">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>9</v>
-      </c>
-      <c r="B80" t="s">
-        <v>17</v>
-      </c>
-      <c r="C80">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>9</v>
-      </c>
-      <c r="B81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>